<commit_message>
Added `LED Matrix Bit Pattern`
</commit_message>
<xml_diff>
--- a/labs/labs11-IntroToMicrocontroller/files/LED_Metrix.xlsx
+++ b/labs/labs11-IntroToMicrocontroller/files/LED_Metrix.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tae/Projects/PhysicalComputing-167/labs/labs11-IntroToMicrocontroller/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27BB1B0-47B4-C148-AB9D-764D5354BF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D500886-7611-9741-9402-AA7503021AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10860" yWindow="500" windowWidth="27540" windowHeight="19960" xr2:uid="{3DC0D921-DEEB-6445-9BE5-4C22741F5A71}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Backup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>index</t>
   </si>
@@ -237,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -278,6 +279,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061072F4-F705-A647-BB78-F849788E4271}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="282" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +713,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -762,7 +766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -772,11 +776,11 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -787,11 +791,11 @@
       <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1</v>
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
       </c>
       <c r="K3" s="3">
         <v>1</v>
@@ -804,18 +808,18 @@
       </c>
       <c r="O3" s="3" t="str">
         <f t="shared" ref="O3:O9" si="0">BIN2HEX(_xlfn.CONCAT(B3, C3, D3, E3))</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P3" s="3" t="str">
         <f t="shared" ref="P3:P9" si="1">BIN2HEX(_xlfn.CONCAT(F3, G3, H3, I3))</f>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="Q3" s="3" t="str">
         <f t="shared" ref="Q3:Q9" si="2">BIN2HEX(_xlfn.CONCAT(J3, K3, L3, M3))</f>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -825,11 +829,11 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -840,11 +844,11 @@
       <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1</v>
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -857,18 +861,18 @@
       </c>
       <c r="O4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F</v>
+        <v>E</v>
       </c>
       <c r="Q4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -881,20 +885,20 @@
       <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
@@ -910,18 +914,18 @@
       </c>
       <c r="O5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -937,14 +941,14 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -967,7 +971,7 @@
       </c>
       <c r="P6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="3" t="str">
         <f t="shared" si="2"/>
@@ -993,8 +997,8 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="3">
-        <v>1</v>
+      <c r="G7" s="8">
+        <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -1020,7 +1024,7 @@
       </c>
       <c r="P7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>E</v>
+        <v>A</v>
       </c>
       <c r="Q7" s="3" t="str">
         <f t="shared" si="2"/>
@@ -1152,33 +1156,612 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="str">
         <f>"0x" &amp; _xlfn.CONCAT(O2:Q2,O3:Q3,O4:P4)</f>
-        <v>0x3187BC7F</v>
+        <v>0x3184A44E</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="str">
         <f>"0x" &amp; _xlfn.CONCAT(Q4,O5:Q5,O6:Q6,O7)</f>
-        <v>0xC3F81F00</v>
+        <v>0x42081100</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6" t="str">
         <f>"0x" &amp; _xlfn.CONCAT(P7:Q7,O8:Q8,O9:Q9)</f>
-        <v>0xE0040000</v>
+        <v>0xA0040000</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
+      <c r="O12" s="15"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="str">
+        <f>"{" &amp; _xlfn.TEXTJOIN(", ", 1, B12:M12) &amp; "}"</f>
+        <v>{0x3184A44E, 0x42081100, 0xA0040000}</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B13:M13"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="B11:M11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="J12:M12"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2:M9">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA67D77-3EA0-DD48-906C-159E4081291C}">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView zoomScale="282" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="13" width="3" customWidth="1"/>
+    <col min="15" max="17" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3" t="str">
+        <f>BIN2HEX(_xlfn.CONCAT(B2, C2, D2, E2))</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="3" t="str">
+        <f>BIN2HEX(_xlfn.CONCAT(F2, G2, H2, I2))</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3" t="str">
+        <f>BIN2HEX(_xlfn.CONCAT(J2, K2, L2, M2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="str">
+        <f t="shared" ref="O3:O9" si="0">BIN2HEX(_xlfn.CONCAT(B3, C3, D3, E3))</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="str">
+        <f t="shared" ref="P3:P9" si="1">BIN2HEX(_xlfn.CONCAT(F3, G3, H3, I3))</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3" t="str">
+        <f t="shared" ref="Q3:Q9" si="2">BIN2HEX(_xlfn.CONCAT(J3, K3, L3, M3))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="str">
+        <f>"0x" &amp; _xlfn.CONCAT(O2:Q2,O3:Q3,O4:P4)</f>
+        <v>0x00000000</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="str">
+        <f>"0x" &amp; _xlfn.CONCAT(Q4,O5:Q5,O6:Q6,O7)</f>
+        <v>0x00000000</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="str">
+        <f>"0x" &amp; _xlfn.CONCAT(P7:Q7,O8:Q8,O9:Q9)</f>
+        <v>0x00000000</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="O12" s="15"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="str">
+        <f>"{" &amp; _xlfn.TEXTJOIN(", ", 1, B12:M12) &amp; "}"</f>
+        <v>{0x00000000, 0x00000000, 0x00000000}</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="B13:M13"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:M9">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>